<commit_message>
Fix replacement type for TR3, TR6
</commit_message>
<xml_diff>
--- a/docs/zxspectrum-bom.xlsx
+++ b/docs/zxspectrum-bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="232">
   <si>
     <t>Qty</t>
   </si>
@@ -157,7 +157,16 @@
     <t>637-BC548C</t>
   </si>
   <si>
-    <t>TR1 TR2 TR3 TR6</t>
+    <t>TR1 TR2</t>
+  </si>
+  <si>
+    <t>Replacement: MPS2369</t>
+  </si>
+  <si>
+    <t>863-MPS2369</t>
+  </si>
+  <si>
+    <t>TR3 TR6</t>
   </si>
   <si>
     <t>ZTX650</t>
@@ -1153,7 +1162,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1389,7 +1398,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>43</v>
@@ -1409,22 +1418,22 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
         <v>48</v>
-      </c>
-      <c r="C16" t="s">
-        <v>49</v>
       </c>
       <c r="D16" t="s">
         <v>45</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1432,19 +1441,19 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
         <v>52</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
       </c>
       <c r="D17" t="s">
         <v>45</v>
       </c>
       <c r="E17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1452,78 +1461,81 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
         <v>56</v>
-      </c>
-      <c r="C18" t="s">
-        <v>49</v>
       </c>
       <c r="D18" t="s">
         <v>45</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
         <v>45</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="3" t="s">
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="2" t="s">
+      <c r="C20" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21">
-        <v>12</v>
-      </c>
-      <c r="B21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="A21" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7">
       <c r="A22">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
         <v>67</v>
-      </c>
-      <c r="D22" t="s">
-        <v>64</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>68</v>
@@ -1540,7 +1552,7 @@
         <v>70</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>71</v>
@@ -1550,42 +1562,42 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="2" t="s">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="D24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25">
-        <v>2</v>
-      </c>
-      <c r="B25" t="s">
-        <v>74</v>
-      </c>
-      <c r="D25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25" s="4" t="s">
+      <c r="A25" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7">
       <c r="A26">
         <v>2</v>
       </c>
       <c r="B26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" t="s">
         <v>78</v>
-      </c>
-      <c r="D26" t="s">
-        <v>75</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>79</v>
@@ -1596,13 +1608,13 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
         <v>81</v>
       </c>
       <c r="D27" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>82</v>
@@ -1613,13 +1625,13 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28" t="s">
         <v>84</v>
       </c>
       <c r="D28" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>85</v>
@@ -1636,7 +1648,7 @@
         <v>87</v>
       </c>
       <c r="D29" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>88</v>
@@ -1647,13 +1659,13 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
         <v>90</v>
       </c>
       <c r="D30" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>91</v>
@@ -1664,13 +1676,13 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" t="s">
         <v>93</v>
       </c>
       <c r="D31" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>94</v>
@@ -1681,13 +1693,13 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="B32" t="s">
         <v>96</v>
       </c>
       <c r="D32" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>97</v>
@@ -1698,13 +1710,13 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B33" t="s">
         <v>99</v>
       </c>
       <c r="D33" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>100</v>
@@ -1715,13 +1727,13 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
         <v>102</v>
       </c>
       <c r="D34" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>103</v>
@@ -1732,13 +1744,13 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
         <v>105</v>
       </c>
       <c r="D35" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>106</v>
@@ -1749,33 +1761,33 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B36" t="s">
         <v>108</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D36" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" s="4" t="s">
+      <c r="F36" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" t="s">
         <v>112</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>113</v>
@@ -1785,42 +1797,42 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="2" t="s">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
         <v>115</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="D38" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39">
-        <v>1</v>
-      </c>
-      <c r="B39" t="s">
-        <v>116</v>
-      </c>
-      <c r="D39" t="s">
-        <v>64</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F39" s="3" t="s">
+      <c r="A39" s="2" t="s">
         <v>118</v>
       </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
     </row>
     <row r="40" spans="1:7">
       <c r="A40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B40" t="s">
         <v>119</v>
       </c>
       <c r="D40" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>120</v>
@@ -1831,13 +1843,13 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B41" t="s">
         <v>122</v>
       </c>
       <c r="D41" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>123</v>
@@ -1854,7 +1866,7 @@
         <v>125</v>
       </c>
       <c r="D42" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>126</v>
@@ -1871,7 +1883,7 @@
         <v>128</v>
       </c>
       <c r="D43" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>129</v>
@@ -1888,7 +1900,7 @@
         <v>131</v>
       </c>
       <c r="D44" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>132</v>
@@ -1899,13 +1911,13 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B45" t="s">
         <v>134</v>
       </c>
       <c r="D45" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>135</v>
@@ -1916,13 +1928,13 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B46" t="s">
         <v>137</v>
       </c>
       <c r="D46" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>138</v>
@@ -1933,13 +1945,13 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
         <v>140</v>
       </c>
       <c r="D47" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>141</v>
@@ -1950,13 +1962,13 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B48" t="s">
         <v>143</v>
       </c>
       <c r="D48" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>144</v>
@@ -1967,13 +1979,13 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B49" t="s">
         <v>146</v>
       </c>
       <c r="D49" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>147</v>
@@ -1984,13 +1996,13 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B50" t="s">
         <v>149</v>
       </c>
       <c r="D50" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>150</v>
@@ -2001,33 +2013,33 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B51" t="s">
         <v>152</v>
       </c>
       <c r="D51" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D52" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>156</v>
@@ -2035,13 +2047,13 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B53" t="s">
         <v>157</v>
       </c>
       <c r="D53" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E53" s="4" t="s">
         <v>158</v>
@@ -2052,13 +2064,13 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B54" t="s">
         <v>160</v>
       </c>
       <c r="D54" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E54" s="4" t="s">
         <v>161</v>
@@ -2075,7 +2087,7 @@
         <v>163</v>
       </c>
       <c r="D55" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>164</v>
@@ -2092,7 +2104,7 @@
         <v>166</v>
       </c>
       <c r="D56" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>167</v>
@@ -2103,13 +2115,13 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B57" t="s">
         <v>169</v>
       </c>
       <c r="D57" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>170</v>
@@ -2120,13 +2132,13 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B58" t="s">
         <v>172</v>
       </c>
       <c r="D58" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>173</v>
@@ -2137,13 +2149,13 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B59" t="s">
         <v>175</v>
       </c>
       <c r="D59" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>176</v>
@@ -2160,7 +2172,7 @@
         <v>178</v>
       </c>
       <c r="D60" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>179</v>
@@ -2170,29 +2182,32 @@
       </c>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="2" t="s">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61" t="s">
         <v>181</v>
       </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
+      <c r="D61" t="s">
+        <v>67</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62">
-        <v>1</v>
-      </c>
-      <c r="B62" t="s">
-        <v>182</v>
-      </c>
-      <c r="D62" t="s">
-        <v>183</v>
-      </c>
-      <c r="F62" s="3" t="s">
+      <c r="A62" s="2" t="s">
         <v>184</v>
       </c>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
     </row>
     <row r="63" spans="1:7">
       <c r="A63">
@@ -2202,9 +2217,6 @@
         <v>185</v>
       </c>
       <c r="D63" t="s">
-        <v>183</v>
-      </c>
-      <c r="E63" s="4" t="s">
         <v>186</v>
       </c>
       <c r="F63" s="3" t="s">
@@ -2212,42 +2224,42 @@
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="2" t="s">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
         <v>188</v>
       </c>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
+      <c r="D64" t="s">
+        <v>186</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65">
-        <v>1</v>
-      </c>
-      <c r="B65" t="s">
-        <v>189</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>190</v>
-      </c>
+      <c r="A65" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
     </row>
     <row r="66" spans="1:7">
       <c r="A66">
         <v>1</v>
       </c>
       <c r="B66" t="s">
-        <v>191</v>
-      </c>
-      <c r="C66" t="s">
         <v>192</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2255,10 +2267,16 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
+        <v>194</v>
+      </c>
+      <c r="C67" t="s">
         <v>195</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>196</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -2266,29 +2284,29 @@
         <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>197</v>
+        <v>198</v>
+      </c>
+      <c r="C68" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>198</v>
-      </c>
-      <c r="C69" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B70" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C70" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2296,12 +2314,9 @@
         <v>1</v>
       </c>
       <c r="B71" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C71" t="s">
-        <v>203</v>
-      </c>
-      <c r="E71" s="4" t="s">
         <v>204</v>
       </c>
     </row>
@@ -2329,84 +2344,78 @@
       <c r="C73" t="s">
         <v>209</v>
       </c>
+      <c r="E73" s="4" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74" t="s">
+        <v>211</v>
+      </c>
+      <c r="C74" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75">
         <v>4</v>
       </c>
-      <c r="B74" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="A75" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
-      <c r="G75" s="2"/>
+      <c r="B75" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="76" spans="1:7">
-      <c r="A76">
-        <v>2</v>
-      </c>
-      <c r="B76" t="s">
-        <v>212</v>
-      </c>
-      <c r="C76" t="s">
-        <v>213</v>
-      </c>
-      <c r="D76" t="s">
-        <v>36</v>
-      </c>
-      <c r="E76" s="4" t="s">
+      <c r="A76" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="F76" s="3" t="s">
-        <v>215</v>
-      </c>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
     </row>
     <row r="77" spans="1:7">
       <c r="A77">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B77" t="s">
+        <v>215</v>
+      </c>
+      <c r="C77" t="s">
         <v>216</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
+        <v>36</v>
+      </c>
+      <c r="E77" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D77" t="s">
-        <v>19</v>
-      </c>
-      <c r="E77" s="4" t="s">
+      <c r="F77" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B78" t="s">
+        <v>219</v>
+      </c>
+      <c r="C78" t="s">
         <v>220</v>
       </c>
-      <c r="C78" t="s">
-        <v>29</v>
-      </c>
       <c r="D78" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="E78" s="4" t="s">
         <v>221</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>31</v>
+        <v>222</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2414,44 +2423,64 @@
         <v>1</v>
       </c>
       <c r="B79" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C79" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D79" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B80" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C80" t="s">
-        <v>225</v>
+        <v>22</v>
       </c>
       <c r="D80" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E80" s="4" t="s">
         <v>226</v>
       </c>
       <c r="F80" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81">
+        <v>2</v>
+      </c>
+      <c r="B81" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" ht="60" customHeight="1">
-      <c r="A82" s="5" t="s">
+      <c r="C81" t="s">
         <v>228</v>
+      </c>
+      <c r="D81" t="s">
+        <v>12</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="60" customHeight="1">
+      <c r="A83" s="5" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2459,13 +2488,13 @@
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A61:G61"/>
-    <mergeCell ref="A64:G64"/>
-    <mergeCell ref="A75:G75"/>
-    <mergeCell ref="A82:G82"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A62:G62"/>
+    <mergeCell ref="A65:G65"/>
+    <mergeCell ref="A76:G76"/>
+    <mergeCell ref="A83:G83"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1"/>
@@ -2477,10 +2506,10 @@
     <hyperlink ref="E17" r:id="rId7"/>
     <hyperlink ref="E18" r:id="rId8"/>
     <hyperlink ref="E19" r:id="rId9"/>
-    <hyperlink ref="E21" r:id="rId10"/>
+    <hyperlink ref="E20" r:id="rId10"/>
     <hyperlink ref="E22" r:id="rId11"/>
     <hyperlink ref="E23" r:id="rId12"/>
-    <hyperlink ref="E25" r:id="rId13"/>
+    <hyperlink ref="E24" r:id="rId13"/>
     <hyperlink ref="E26" r:id="rId14"/>
     <hyperlink ref="E27" r:id="rId15"/>
     <hyperlink ref="E28" r:id="rId16"/>
@@ -2493,7 +2522,7 @@
     <hyperlink ref="E35" r:id="rId23"/>
     <hyperlink ref="E36" r:id="rId24"/>
     <hyperlink ref="E37" r:id="rId25"/>
-    <hyperlink ref="E39" r:id="rId26"/>
+    <hyperlink ref="E38" r:id="rId26"/>
     <hyperlink ref="E40" r:id="rId27"/>
     <hyperlink ref="E41" r:id="rId28"/>
     <hyperlink ref="E42" r:id="rId29"/>
@@ -2515,16 +2544,17 @@
     <hyperlink ref="E58" r:id="rId45"/>
     <hyperlink ref="E59" r:id="rId46"/>
     <hyperlink ref="E60" r:id="rId47"/>
-    <hyperlink ref="E63" r:id="rId48"/>
-    <hyperlink ref="E65" r:id="rId49"/>
+    <hyperlink ref="E61" r:id="rId48"/>
+    <hyperlink ref="E64" r:id="rId49"/>
     <hyperlink ref="E66" r:id="rId50"/>
-    <hyperlink ref="E71" r:id="rId51"/>
+    <hyperlink ref="E67" r:id="rId51"/>
     <hyperlink ref="E72" r:id="rId52"/>
-    <hyperlink ref="E76" r:id="rId53"/>
+    <hyperlink ref="E73" r:id="rId53"/>
     <hyperlink ref="E77" r:id="rId54"/>
     <hyperlink ref="E78" r:id="rId55"/>
     <hyperlink ref="E79" r:id="rId56"/>
     <hyperlink ref="E80" r:id="rId57"/>
+    <hyperlink ref="E81" r:id="rId58"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>